<commit_message>
Talk is not talk...
</commit_message>
<xml_diff>
--- a/markdown_generator/talks.xlsx
+++ b/markdown_generator/talks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlie/Documents/charlieduclut.github.io/markdown_generator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlie/charlieduclut.github.io/markdown_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD88814-818C-7F4F-9C38-4BD11546DBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4235258A-BB5F-5047-8EE2-D308EF012729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="1460" windowWidth="24640" windowHeight="13440" xr2:uid="{F09A7C8F-8E58-E542-BD9D-52A82FED7577}"/>
   </bookViews>
@@ -310,9 +310,6 @@
     <t>Physics Meets Biology</t>
   </si>
   <si>
-    <t>Invited Talk</t>
-  </si>
-  <si>
     <t>inv-talk-1</t>
   </si>
   <si>
@@ -377,6 +374,9 @@
   </si>
   <si>
     <t>New frontiers in liquid matter</t>
+  </si>
+  <si>
+    <t>Invited talk</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -739,7 +739,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -750,7 +750,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -790,10 +790,10 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
         <v>92</v>
-      </c>
-      <c r="C2" t="s">
-        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>25</v>
@@ -807,22 +807,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" s="1">
         <v>44907</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -842,7 +842,7 @@
         <v>42397</v>
       </c>
       <c r="F4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -967,7 +967,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -976,7 +976,7 @@
         <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E11" s="1">
         <v>44749</v>
@@ -1147,13 +1147,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D20" t="s">
         <v>50</v>
@@ -1167,56 +1167,56 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B21" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E21" s="3">
         <v>44589</v>
       </c>
       <c r="F21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B22" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E22" s="3">
         <v>44608</v>
       </c>
       <c r="F22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B23" t="s">
         <v>38</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E23" s="3">
         <v>44614</v>
@@ -1227,16 +1227,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B24" t="s">
         <v>38</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E24" s="3">
         <v>44844</v>
@@ -1276,7 +1276,7 @@
         <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E26" s="3">
         <v>42583</v>
@@ -1316,7 +1316,7 @@
         <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E28" s="3">
         <v>43313</v>

</xml_diff>

<commit_message>
2023-10-24 updated talk list
</commit_message>
<xml_diff>
--- a/markdown_generator/talks.xlsx
+++ b/markdown_generator/talks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlie/charlieduclut.github.io/markdown_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25083EF5-4FAC-7F44-8D05-2D652FC268D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E67C25-43F7-5248-8214-6B3AFCA50F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="1460" windowWidth="24640" windowHeight="13440" xr2:uid="{F09A7C8F-8E58-E542-BD9D-52A82FED7577}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="133">
   <si>
     <t>title</t>
   </si>
@@ -419,6 +419,18 @@
   </si>
   <si>
     <t>poster-13</t>
+  </si>
+  <si>
+    <t>talk-11</t>
+  </si>
+  <si>
+    <t>Rice Global Paris Center, Paris, France</t>
+  </si>
+  <si>
+    <t>Hydraulic and electric properties of tissues</t>
+  </si>
+  <si>
+    <t>Physics meets Biology</t>
   </si>
 </sst>
 </file>
@@ -789,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C56962E-EF5E-A549-B915-DB3E499CC727}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1069,42 +1081,42 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="3">
-        <v>42824</v>
+        <v>132</v>
+      </c>
+      <c r="E14" s="1">
+        <v>45223</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E15" s="3">
-        <v>43837</v>
+        <v>42824</v>
       </c>
       <c r="F15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1115,16 +1127,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E16" s="3">
-        <v>43839</v>
+        <v>43837</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1135,76 +1147,76 @@
         <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E17" s="3">
-        <v>43845</v>
+        <v>43839</v>
       </c>
       <c r="F17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>53</v>
+      <c r="C18" t="s">
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E18" s="3">
-        <v>43921</v>
+        <v>43845</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E19" s="3">
-        <v>44118</v>
+        <v>43921</v>
       </c>
       <c r="F19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E20" s="3">
-        <v>44137</v>
+        <v>44118</v>
       </c>
       <c r="F20" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1215,36 +1227,36 @@
         <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E21" s="3">
-        <v>44145</v>
+        <v>44137</v>
       </c>
       <c r="F21" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="E22" s="3">
-        <v>44543</v>
+        <v>44145</v>
       </c>
       <c r="F22" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1255,16 +1267,16 @@
         <v>38</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D23" t="s">
-        <v>107</v>
+        <v>50</v>
       </c>
       <c r="E23" s="3">
-        <v>44589</v>
+        <v>44543</v>
       </c>
       <c r="F23" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1275,16 +1287,16 @@
         <v>38</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E24" s="3">
-        <v>44608</v>
+        <v>44589</v>
       </c>
       <c r="F24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1295,33 +1307,33 @@
         <v>38</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="E25" s="3">
-        <v>44614</v>
+        <v>44608</v>
       </c>
       <c r="F25" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B26" t="s">
         <v>38</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D26" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="E26" s="3">
-        <v>44844</v>
+        <v>44614</v>
       </c>
       <c r="F26" t="s">
         <v>65</v>
@@ -1329,42 +1341,42 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" t="s">
-        <v>68</v>
+        <v>38</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="E27" s="3">
-        <v>41050</v>
+        <v>44844</v>
       </c>
       <c r="F27" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
         <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D28" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="E28" s="3">
-        <v>42583</v>
+        <v>41050</v>
       </c>
       <c r="F28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1375,36 +1387,36 @@
         <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="E29" s="3">
-        <v>42775</v>
+        <v>42583</v>
       </c>
       <c r="F29" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
         <v>67</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D30" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="E30" s="3">
-        <v>43313</v>
+        <v>42775</v>
       </c>
       <c r="F30" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1415,16 +1427,16 @@
         <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D31" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="E31" s="3">
-        <v>43586</v>
+        <v>43313</v>
       </c>
       <c r="F31" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1435,16 +1447,16 @@
         <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E32" s="3">
-        <v>43649</v>
+        <v>43586</v>
       </c>
       <c r="F32" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1455,16 +1467,16 @@
         <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E33" s="3">
-        <v>43759</v>
+        <v>43649</v>
       </c>
       <c r="F33" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1475,33 +1487,33 @@
         <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E34" s="3">
-        <v>44125</v>
+        <v>43759</v>
       </c>
       <c r="F34" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B35" t="s">
         <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E35" s="3">
-        <v>44354</v>
+        <v>44125</v>
       </c>
       <c r="F35" t="s">
         <v>30</v>
@@ -1515,13 +1527,13 @@
         <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E36" s="3">
-        <v>44403</v>
+        <v>44354</v>
       </c>
       <c r="F36" t="s">
         <v>30</v>
@@ -1529,22 +1541,22 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>124</v>
+        <v>27</v>
       </c>
       <c r="B37" t="s">
         <v>67</v>
       </c>
       <c r="C37" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="D37" t="s">
-        <v>125</v>
-      </c>
-      <c r="E37" s="1">
-        <v>44656</v>
+        <v>91</v>
+      </c>
+      <c r="E37" s="3">
+        <v>44403</v>
       </c>
       <c r="F37" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1555,35 +1567,55 @@
         <v>67</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E38" s="1">
-        <v>44740</v>
+        <v>44656</v>
       </c>
       <c r="F38" t="s">
-        <v>127</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B39" t="s">
         <v>67</v>
       </c>
       <c r="C39" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" t="s">
+        <v>126</v>
+      </c>
+      <c r="E39" s="1">
+        <v>44740</v>
+      </c>
+      <c r="F39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" t="s">
         <v>128</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>122</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E40" s="1">
         <v>45041</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>